<commit_message>
added table with priviliges of user groups to document 'User Views'
</commit_message>
<xml_diff>
--- a/Docs/Corvin/Datenkatalog.xlsx
+++ b/Docs/Corvin/Datenkatalog.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Benutzer\Tobi\Dokumente HDD\Hochschule Esslingen\Semester 6\Informationssysteme\InfoSys-Lab\Docs\Corvin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Desktop\hs-esslingen\Unterrichtsfächer\7. Semester\Infosys\GitRepo\InfoSys-Lab\Docs\Corvin\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9045" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9045"/>
   </bookViews>
   <sheets>
     <sheet name="Entity" sheetId="1" r:id="rId1"/>
     <sheet name="Relations" sheetId="2" r:id="rId2"/>
     <sheet name="Attributes" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="102">
   <si>
     <t>Name</t>
   </si>
@@ -329,6 +329,9 @@
   </si>
   <si>
     <t>yes?????</t>
+  </si>
+  <si>
+    <t>Muss eine Historie für Professoren geführt werden, in welchem Semester Sie wie viele SWS geleistet haben?</t>
   </si>
 </sst>
 </file>
@@ -683,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,6 +795,11 @@
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -968,7 +976,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>

</xml_diff>